<commit_message>
Added checklist from Excel
</commit_message>
<xml_diff>
--- a/unit_tests.xlsx
+++ b/unit_tests.xlsx
@@ -9,17 +9,18 @@
   <sheets>
     <sheet name="headers" sheetId="1" r:id="rId1"/>
     <sheet name="items" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="checklist" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="tblItems">items!$A$1:$D$9</definedName>
+    <definedName name="exChkLst">checklist!$A$1:$D$2</definedName>
+    <definedName name="exItems">items!$A$1:$D$9</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>chklst_header_text</t>
   </si>
@@ -70,6 +71,27 @@
   </si>
   <si>
     <t>All unit tests are complete.</t>
+  </si>
+  <si>
+    <t>chklst_name</t>
+  </si>
+  <si>
+    <t>template_id</t>
+  </si>
+  <si>
+    <t>area_code</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>Panic Plan</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>This Panic Pan is based on science fiction.</t>
   </si>
 </sst>
 </file>
@@ -469,7 +491,7 @@
   <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,12 +920,49 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>